<commit_message>
GBDS FEBRUARY FILES 2026 | fliqlo@GBDS
</commit_message>
<xml_diff>
--- a/GBDS FEBRUARY FILES 2026/CSR MONTH OF FEBRUARY 2026.xlsx
+++ b/GBDS FEBRUARY FILES 2026/CSR MONTH OF FEBRUARY 2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS FEBRUARY FILES 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2448C08-621A-46F6-B443-656BA63AA2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D502AC23-B702-4853-8123-A2AF13757780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="16" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | FEBRUARY" sheetId="902" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="91">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -317,6 +317,30 @@
   </si>
   <si>
     <t>DATE _______________________________</t>
+  </si>
+  <si>
+    <t>7/23B</t>
+  </si>
+  <si>
+    <t>2/2B</t>
+  </si>
+  <si>
+    <t>10/1B</t>
+  </si>
+  <si>
+    <t>10/16B</t>
+  </si>
+  <si>
+    <t>6/7B</t>
+  </si>
+  <si>
+    <t>4/9B</t>
+  </si>
+  <si>
+    <t>5/20B</t>
+  </si>
+  <si>
+    <t>12/4B</t>
   </si>
 </sst>
 </file>
@@ -1191,39 +1215,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1231,12 +1222,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1273,6 +1258,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3752,58 +3776,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -3846,13 +3870,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -3877,7 +3901,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -3902,8 +3926,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -3929,7 +3953,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -3955,7 +3979,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -3981,7 +4005,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -4006,11 +4030,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -4035,12 +4059,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -5359,10 +5383,10 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
@@ -5370,48 +5394,48 @@
       <c r="Z33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
       <c r="Z34" s="32"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -5457,7 +5481,7 @@
       <c r="Q35" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="87"/>
+      <c r="R35" s="76"/>
       <c r="S35" s="70"/>
       <c r="T35" s="70"/>
       <c r="U35" s="40"/>
@@ -5510,7 +5534,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -5614,11 +5638,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -5643,12 +5667,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -6976,47 +7000,47 @@
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="84"/>
-      <c r="T34" s="84"/>
-      <c r="U34" s="84"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="101"/>
       <c r="V34" s="72"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
     </row>
     <row r="35" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -7059,7 +7083,7 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
       <c r="R35" s="70"/>
@@ -7115,7 +7139,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -7219,11 +7243,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -7248,12 +7272,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -8569,58 +8593,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -8663,13 +8687,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -8694,7 +8718,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -8719,8 +8743,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -8746,7 +8770,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -8772,7 +8796,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -8798,7 +8822,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -8823,11 +8847,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -8852,12 +8876,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -10171,58 +10195,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -10265,13 +10289,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -10296,7 +10320,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -10321,8 +10345,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -10348,7 +10372,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -10374,7 +10398,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -10400,7 +10424,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -10425,11 +10449,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -10454,12 +10478,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -11778,10 +11802,10 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
@@ -11789,48 +11813,48 @@
       <c r="Z33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
       <c r="Z34" s="32"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -11876,7 +11900,7 @@
       <c r="Q35" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="87"/>
+      <c r="R35" s="76"/>
       <c r="S35" s="70"/>
       <c r="T35" s="70"/>
       <c r="U35" s="40"/>
@@ -11929,7 +11953,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -12033,11 +12057,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -12062,12 +12086,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -13395,47 +13419,47 @@
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="84"/>
-      <c r="T34" s="84"/>
-      <c r="U34" s="84"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="101"/>
       <c r="V34" s="72"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
     </row>
     <row r="35" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -13478,7 +13502,7 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
       <c r="R35" s="70"/>
@@ -13534,7 +13558,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -13638,11 +13662,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -13667,12 +13691,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -13726,7 +13750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BC1B7F-7988-41AD-818A-09552FB189F9}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -14988,58 +15012,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -15082,13 +15106,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -15113,7 +15137,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -15138,8 +15162,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -15165,7 +15189,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -15191,7 +15215,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -15217,7 +15241,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -15242,11 +15266,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -15271,12 +15295,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -16605,48 +16629,48 @@
       <c r="Z33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="74" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="75"/>
-      <c r="S34" s="75"/>
-      <c r="T34" s="76"/>
-      <c r="U34" s="77" t="s">
+      <c r="P34" s="90"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="90"/>
+      <c r="S34" s="90"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="V34" s="78"/>
-      <c r="W34" s="78"/>
-      <c r="X34" s="78"/>
-      <c r="Y34" s="79"/>
+      <c r="V34" s="93"/>
+      <c r="W34" s="93"/>
+      <c r="X34" s="93"/>
+      <c r="Y34" s="94"/>
       <c r="Z34" s="32"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -16881,13 +16905,13 @@
       <c r="R42" s="68"/>
       <c r="S42" s="68"/>
       <c r="T42" s="46"/>
-      <c r="U42" s="80" t="s">
+      <c r="U42" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="V42" s="80"/>
-      <c r="W42" s="80"/>
-      <c r="X42" s="80"/>
-      <c r="Y42" s="80"/>
+      <c r="V42" s="95"/>
+      <c r="W42" s="95"/>
+      <c r="X42" s="95"/>
+      <c r="Y42" s="95"/>
     </row>
     <row r="43" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -18262,10 +18286,10 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
@@ -18273,48 +18297,48 @@
       <c r="Z33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
       <c r="Z34" s="32"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -18360,7 +18384,7 @@
       <c r="Q35" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="87"/>
+      <c r="R35" s="76"/>
       <c r="S35" s="70"/>
       <c r="T35" s="70"/>
       <c r="U35" s="40"/>
@@ -18437,7 +18461,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -18541,11 +18565,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -18594,12 +18618,12 @@
       <c r="Q42" s="46">
         <v>34</v>
       </c>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -18633,14 +18657,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="R42:U42"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="R42:U42"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
@@ -19993,47 +20017,47 @@
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="84"/>
-      <c r="T34" s="84"/>
-      <c r="U34" s="84"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="101"/>
       <c r="V34" s="72"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
     </row>
     <row r="35" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -20076,7 +20100,7 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
       <c r="R35" s="70"/>
@@ -20148,7 +20172,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -20252,11 +20276,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -20297,12 +20321,12 @@
       <c r="Q42" s="46">
         <v>18</v>
       </c>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -20336,14 +20360,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="R42:U42"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="R42:U42"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
@@ -21672,58 +21696,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -21766,13 +21790,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -21817,7 +21841,7 @@
       <c r="Q36" s="46">
         <v>7</v>
       </c>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -21842,8 +21866,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -21869,7 +21893,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -21895,7 +21919,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -21921,7 +21945,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -21946,11 +21970,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -21995,12 +22019,12 @@
       <c r="Q42" s="46">
         <v>7</v>
       </c>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -22034,14 +22058,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:U34"/>
+    <mergeCell ref="R42:U42"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:U34"/>
-    <mergeCell ref="R42:U42"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
@@ -23314,58 +23338,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -23408,13 +23432,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -23439,7 +23463,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -23464,8 +23488,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -23491,7 +23515,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -23517,7 +23541,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -23543,7 +23567,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -23568,11 +23592,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -23597,12 +23621,12 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -24020,17 +24044,29 @@
       <c r="W7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="X7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15">
+        <v>2</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -24043,11 +24079,17 @@
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
+      <c r="U8" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
+      <c r="W8" s="15">
+        <v>1</v>
+      </c>
       <c r="X8" s="62"/>
-      <c r="Y8" s="16"/>
+      <c r="Y8" s="16" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -24213,12 +24255,20 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>2</v>
+      </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>83</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -24231,22 +24281,36 @@
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
+      <c r="U15" s="24">
+        <v>0</v>
+      </c>
       <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="W15" s="24">
+        <v>0</v>
+      </c>
       <c r="X15" s="64"/>
-      <c r="Y15" s="25"/>
+      <c r="Y15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
       <c r="D16" s="61"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="F16" s="28">
+        <v>2</v>
+      </c>
+      <c r="G16" s="29">
+        <v>2</v>
+      </c>
+      <c r="H16" s="67" t="s">
+        <v>84</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -24259,11 +24323,17 @@
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
       <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
+      <c r="U16" s="29" t="s">
+        <v>75</v>
+      </c>
       <c r="V16" s="29"/>
-      <c r="W16" s="59"/>
+      <c r="W16" s="59">
+        <v>1</v>
+      </c>
       <c r="X16" s="65"/>
-      <c r="Y16" s="30"/>
+      <c r="Y16" s="30" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -24595,71 +24665,67 @@
     <row r="23" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U23" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="T23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="V23" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="W23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="X23" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
     </row>
     <row r="24" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -24671,16 +24737,24 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>20</v>
+      </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="K24" s="15">
+        <v>10</v>
+      </c>
+      <c r="L24" s="15">
+        <v>327</v>
+      </c>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>10</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -24857,16 +24931,24 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="24">
+        <v>2</v>
+      </c>
+      <c r="L31" s="24">
+        <v>20</v>
+      </c>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>5</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -24885,16 +24967,24 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>20</v>
+      </c>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
+      <c r="K32" s="29">
+        <v>8</v>
+      </c>
+      <c r="L32" s="29">
+        <v>307</v>
+      </c>
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>5</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -24921,10 +25011,10 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
@@ -24932,48 +25022,48 @@
       <c r="Z33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
       <c r="Z34" s="32"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -25019,7 +25109,7 @@
       <c r="Q35" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="87"/>
+      <c r="R35" s="76"/>
       <c r="S35" s="70"/>
       <c r="T35" s="70"/>
       <c r="U35" s="40"/>
@@ -25035,18 +25125,40 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
+      <c r="F36" s="45">
+        <v>313</v>
+      </c>
+      <c r="G36" s="45">
+        <v>2</v>
+      </c>
+      <c r="H36" s="45">
+        <v>1</v>
+      </c>
+      <c r="I36" s="45">
+        <v>5</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>5</v>
+      </c>
+      <c r="L36" s="45">
+        <v>1</v>
+      </c>
+      <c r="M36" s="45">
+        <v>2</v>
+      </c>
+      <c r="N36" s="45">
+        <v>20</v>
+      </c>
+      <c r="O36" s="45">
+        <v>5</v>
+      </c>
       <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="Q36" s="46">
+        <v>10</v>
+      </c>
       <c r="R36" s="71"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
@@ -25072,7 +25184,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -25176,11 +25288,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -25193,24 +25305,46 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
+      <c r="F42" s="45">
+        <v>313</v>
+      </c>
+      <c r="G42" s="45">
+        <v>2</v>
+      </c>
+      <c r="H42" s="45">
+        <v>1</v>
+      </c>
+      <c r="I42" s="45">
+        <v>5</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>5</v>
+      </c>
+      <c r="L42" s="45">
+        <v>1</v>
+      </c>
+      <c r="M42" s="45">
+        <v>2</v>
+      </c>
+      <c r="N42" s="45">
+        <v>20</v>
+      </c>
+      <c r="O42" s="45">
+        <v>5</v>
+      </c>
       <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="Q42" s="46">
+        <v>10</v>
+      </c>
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -25274,8 +25408,10 @@
     <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
     <col min="3" max="7" width="5.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="5.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="5.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.140625" style="2" customWidth="1"/>
@@ -25627,17 +25763,27 @@
       <c r="W7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="X7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14">
+        <v>3</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>86</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -25650,11 +25796,17 @@
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
+      <c r="U8" s="15">
+        <v>2</v>
+      </c>
       <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
+      <c r="W8" s="15">
+        <v>2</v>
+      </c>
       <c r="X8" s="62"/>
-      <c r="Y8" s="16"/>
+      <c r="Y8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -25820,12 +25972,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>3</v>
+      </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>87</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -25838,22 +25996,34 @@
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
+      <c r="U15" s="24">
+        <v>2</v>
+      </c>
       <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="W15" s="24">
+        <v>2</v>
+      </c>
       <c r="X15" s="64"/>
-      <c r="Y15" s="25"/>
+      <c r="Y15" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
       <c r="D16" s="61"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="67" t="s">
+        <v>88</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -25866,11 +26036,17 @@
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
       <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
+      <c r="U16" s="29">
+        <v>0</v>
+      </c>
       <c r="V16" s="29"/>
-      <c r="W16" s="59"/>
+      <c r="W16" s="59">
+        <v>0</v>
+      </c>
       <c r="X16" s="65"/>
-      <c r="Y16" s="30"/>
+      <c r="Y16" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -26202,92 +26378,100 @@
     <row r="23" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U23" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="T23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="V23" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="W23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="X23" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
     </row>
     <row r="24" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15">
+        <v>3</v>
+      </c>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>33</v>
+      </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="K24" s="15">
+        <v>10</v>
+      </c>
+      <c r="L24" s="15">
+        <v>277</v>
+      </c>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -26459,21 +26643,33 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>0</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
+      <c r="F31" s="24">
+        <v>3</v>
+      </c>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="24">
+        <v>3</v>
+      </c>
+      <c r="L31" s="24">
+        <v>35</v>
+      </c>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -26487,21 +26683,33 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>1</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="28">
+        <v>0</v>
+      </c>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>33</v>
+      </c>
       <c r="I32" s="29"/>
       <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
+      <c r="K32" s="29">
+        <v>7</v>
+      </c>
+      <c r="L32" s="29">
+        <v>242</v>
+      </c>
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -26538,47 +26746,47 @@
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="84"/>
-      <c r="T34" s="84"/>
-      <c r="U34" s="84"/>
+      <c r="S34" s="101"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="101"/>
       <c r="V34" s="72"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
     </row>
     <row r="35" spans="2:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -26621,7 +26829,7 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
       <c r="R35" s="70"/>
@@ -26640,18 +26848,32 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
+      <c r="F36" s="45">
+        <v>316</v>
+      </c>
+      <c r="G36" s="45">
+        <v>3</v>
+      </c>
+      <c r="H36" s="45">
+        <v>5</v>
+      </c>
       <c r="I36" s="45"/>
       <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
+      <c r="K36" s="45">
+        <v>12</v>
+      </c>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
       <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>4</v>
+      </c>
       <c r="R36" s="71"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
@@ -26677,7 +26899,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
+      <c r="Q37" s="74"/>
       <c r="R37" s="71"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
@@ -26781,11 +27003,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="86"/>
+      <c r="T41" s="86"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -26798,24 +27020,38 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
+      <c r="F42" s="45">
+        <v>316</v>
+      </c>
+      <c r="G42" s="45">
+        <v>3</v>
+      </c>
+      <c r="H42" s="45">
+        <v>5</v>
+      </c>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
+      <c r="K42" s="45">
+        <v>12</v>
+      </c>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
       <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>4</v>
+      </c>
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>
@@ -26869,7 +27105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5682E203-6764-4579-88F5-B53BF296447F}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -27230,17 +27466,27 @@
       <c r="W7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="X7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>3</v>
+      </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15">
+        <v>18</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -27253,9 +27499,15 @@
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
+      <c r="U8" s="15">
+        <v>2</v>
+      </c>
+      <c r="V8" s="15">
+        <v>1</v>
+      </c>
+      <c r="W8" s="15">
+        <v>3</v>
+      </c>
       <c r="X8" s="62"/>
       <c r="Y8" s="16"/>
     </row>
@@ -27424,11 +27676,17 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>89</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -27441,9 +27699,15 @@
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="U15" s="24">
+        <v>2</v>
+      </c>
+      <c r="V15" s="24">
+        <v>0</v>
+      </c>
+      <c r="W15" s="24">
+        <v>0</v>
+      </c>
       <c r="X15" s="64"/>
       <c r="Y15" s="25"/>
     </row>
@@ -27452,11 +27716,17 @@
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>2</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>2</v>
+      </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="67" t="s">
+        <v>90</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -27469,9 +27739,15 @@
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
       <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="59"/>
+      <c r="U16" s="29">
+        <v>0</v>
+      </c>
+      <c r="V16" s="29">
+        <v>1</v>
+      </c>
+      <c r="W16" s="59">
+        <v>3</v>
+      </c>
       <c r="X16" s="65"/>
       <c r="Y16" s="30"/>
     </row>
@@ -27805,71 +28081,67 @@
     <row r="23" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="38"/>
       <c r="C23" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U23" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="T23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="V23" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="W23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="X23" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
     </row>
     <row r="24" spans="2:25" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -27879,18 +28151,32 @@
       <c r="C24" s="14"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
+      <c r="H24" s="15">
+        <v>72</v>
+      </c>
+      <c r="I24" s="15">
+        <v>1</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" s="15">
+        <v>15</v>
+      </c>
+      <c r="L24" s="15">
+        <v>528</v>
+      </c>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>10</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -28065,18 +28351,32 @@
       <c r="C31" s="23"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
+      <c r="F31" s="24" t="s">
+        <v>75</v>
+      </c>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
+      <c r="H31" s="24">
+        <v>37</v>
+      </c>
+      <c r="I31" s="24">
+        <v>0</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K31" s="24">
+        <v>11</v>
+      </c>
+      <c r="L31" s="24">
+        <v>114</v>
+      </c>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>10</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -28093,18 +28393,32 @@
       <c r="C32" s="27"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="28">
+        <v>0</v>
+      </c>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
+      <c r="H32" s="29">
+        <v>35</v>
+      </c>
+      <c r="I32" s="29">
+        <v>1</v>
+      </c>
+      <c r="J32" s="29">
+        <v>0</v>
+      </c>
+      <c r="K32" s="29">
+        <v>4</v>
+      </c>
+      <c r="L32" s="29">
+        <v>414</v>
+      </c>
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -28131,58 +28445,58 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
-      <c r="R33" s="92"/>
-      <c r="S33" s="92"/>
-      <c r="T33" s="92"/>
-      <c r="U33" s="92"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="79"/>
+      <c r="T33" s="79"/>
+      <c r="U33" s="79"/>
       <c r="V33" s="32"/>
       <c r="W33" s="32"/>
       <c r="X33" s="32"/>
       <c r="Y33" s="32"/>
     </row>
     <row r="34" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="74" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74" t="s">
+      <c r="G34" s="90"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="74" t="s">
+      <c r="J34" s="90"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="75"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="83" t="s">
+      <c r="M34" s="90"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="77" t="s">
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="90"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="77"/>
       <c r="W34" s="72"/>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
-      <c r="Z34" s="100"/>
+      <c r="Z34" s="87"/>
     </row>
     <row r="35" spans="2:26" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="82"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -28225,13 +28539,13 @@
       <c r="P35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="91" t="s">
+      <c r="Q35" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="94"/>
-      <c r="T35" s="94"/>
-      <c r="U35" s="95"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="82"/>
       <c r="V35" s="40"/>
       <c r="W35" s="40"/>
       <c r="X35" s="40"/>
@@ -28256,7 +28570,7 @@
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="96"/>
+      <c r="R36" s="83"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="73"/>
@@ -28281,8 +28595,8 @@
       <c r="N37" s="51"/>
       <c r="O37" s="51"/>
       <c r="P37" s="51"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="96"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="83"/>
       <c r="S37" s="71"/>
       <c r="T37" s="71"/>
       <c r="U37" s="73"/>
@@ -28308,7 +28622,7 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="96"/>
+      <c r="R38" s="83"/>
       <c r="S38" s="71"/>
       <c r="T38" s="71"/>
       <c r="U38" s="73"/>
@@ -28334,7 +28648,7 @@
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="21"/>
-      <c r="R39" s="96"/>
+      <c r="R39" s="83"/>
       <c r="S39" s="71"/>
       <c r="T39" s="71"/>
       <c r="U39" s="73"/>
@@ -28360,7 +28674,7 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="96"/>
+      <c r="R40" s="83"/>
       <c r="S40" s="71"/>
       <c r="T40" s="71"/>
       <c r="U40" s="73"/>
@@ -28385,11 +28699,11 @@
       <c r="N41" s="42"/>
       <c r="O41" s="42"/>
       <c r="P41" s="42"/>
-      <c r="Q41" s="86"/>
-      <c r="R41" s="97"/>
-      <c r="S41" s="98"/>
-      <c r="T41" s="98"/>
-      <c r="U41" s="99"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="86"/>
       <c r="V41" s="73"/>
       <c r="W41" s="73"/>
       <c r="X41" s="73"/>
@@ -28402,24 +28716,46 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
+      <c r="F42" s="45">
+        <v>429</v>
+      </c>
+      <c r="G42" s="45">
+        <v>17</v>
+      </c>
+      <c r="H42" s="45">
+        <v>2</v>
+      </c>
+      <c r="I42" s="45">
+        <v>8</v>
+      </c>
       <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="88" t="s">
+      <c r="K42" s="45">
+        <v>6</v>
+      </c>
+      <c r="L42" s="45">
+        <v>4</v>
+      </c>
+      <c r="M42" s="45">
+        <v>1</v>
+      </c>
+      <c r="N42" s="45">
+        <v>23</v>
+      </c>
+      <c r="O42" s="45">
+        <v>4</v>
+      </c>
+      <c r="P42" s="45">
+        <v>7</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>20</v>
+      </c>
+      <c r="R42" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="72"/>
       <c r="W42" s="72"/>
       <c r="X42" s="72"/>

</xml_diff>